<commit_message>
Basic fitering and sorting
</commit_message>
<xml_diff>
--- a/Excel worksheet/Basic_Functions_Practice.xlsx
+++ b/Excel worksheet/Basic_Functions_Practice.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zain-Ul-Abadin\Desktop\Excel worksheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zain-Ul-Abadin\Desktop\Data-Analysis-Practice\Excel worksheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3280AB20-7972-40ED-B849-F560AB94F2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C776622D-7B32-489A-A3C1-4C80DE5C6721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{EB0C027C-86E1-46AB-B1DB-C44A33CA8120}"/>
+    <workbookView xWindow="48" yWindow="0" windowWidth="11556" windowHeight="12504" xr2:uid="{EB0C027C-86E1-46AB-B1DB-C44A33CA8120}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$23:$D$24</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
   <si>
     <t>January Month Expenses</t>
   </si>
@@ -45,21 +48,12 @@
     <t>Payment Mode</t>
   </si>
   <si>
-    <t>1st Jan 2026</t>
-  </si>
-  <si>
     <t>Food</t>
   </si>
   <si>
     <t>Zomato</t>
   </si>
   <si>
-    <t>Credit Card</t>
-  </si>
-  <si>
-    <t>2nd Jan 2026</t>
-  </si>
-  <si>
     <t>Dress</t>
   </si>
   <si>
@@ -72,33 +66,21 @@
     <t>Cash</t>
   </si>
   <si>
-    <t>3rd Jan 2026</t>
-  </si>
-  <si>
     <t>Milk</t>
   </si>
   <si>
     <t>Easypaisa</t>
   </si>
   <si>
-    <t>4th Jan 2026</t>
-  </si>
-  <si>
     <t>Chocolate</t>
   </si>
   <si>
-    <t>5th Jan 2026</t>
-  </si>
-  <si>
     <t>Clothes</t>
   </si>
   <si>
     <t>Card</t>
   </si>
   <si>
-    <t>6th Jan 2026</t>
-  </si>
-  <si>
     <t>Bills</t>
   </si>
   <si>
@@ -145,13 +127,50 @@
   </si>
   <si>
     <t>Abbrevation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data sort </t>
+  </si>
+  <si>
+    <t>Essentials</t>
+  </si>
+  <si>
+    <t>Salt and Sugar</t>
+  </si>
+  <si>
+    <t>Diary</t>
+  </si>
+  <si>
+    <t>Chai</t>
+  </si>
+  <si>
+    <t>Shampoo</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Bread and Milk</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>JazzCash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="174" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,8 +200,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,6 +217,54 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -208,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -217,20 +290,168 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="23">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B084"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF70AD47"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B084"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF70AD47"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4472C4"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF70AD47"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4472C4"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF70AD47"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="174" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="174" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -281,16 +502,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C2D2F54-04B6-4DBA-A425-C854A1BBB618}" name="Table1" displayName="Table1" ref="B3:H9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="B3:H9" xr:uid="{3C2D2F54-04B6-4DBA-A425-C854A1BBB618}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C2D2F54-04B6-4DBA-A425-C854A1BBB618}" name="Table1" displayName="Table1" ref="B3:H21" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:H21">
+    <sortCondition ref="C4:C21"/>
+    <sortCondition ref="E4:E21"/>
+  </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{31D8B947-73F6-4CF9-8FEE-1B3F01BA5E62}" name="Date" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{ED180876-860C-449D-A052-7849F4961F6D}" name="Category" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{F08A6562-578F-430E-889C-DA73E7B858EB}" name="Sub Category" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{F534D01F-A85B-4572-A68F-2DE0B7FBD02E}" name="Amount" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{D76E635A-7419-49C9-95B1-E8A713DC36F7}" name="Payment Mode" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{93840539-83D1-4C51-8B4E-388DF557236B}" name="Country Name" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{63C1F6EC-C79F-4A4F-9BE3-769431221B3B}" name="Abbrevation" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{31D8B947-73F6-4CF9-8FEE-1B3F01BA5E62}" name="Date" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{ED180876-860C-449D-A052-7849F4961F6D}" name="Category" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{F08A6562-578F-430E-889C-DA73E7B858EB}" name="Sub Category" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{F534D01F-A85B-4572-A68F-2DE0B7FBD02E}" name="Amount" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{D76E635A-7419-49C9-95B1-E8A713DC36F7}" name="Payment Mode" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{93840539-83D1-4C51-8B4E-388DF557236B}" name="Country Name" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{63C1F6EC-C79F-4A4F-9BE3-769431221B3B}" name="Abbrevation" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{69BDD11D-A29B-4019-A98D-A68DA7D6C355}" name="Table2" displayName="Table2" ref="M3:M12" totalsRowShown="0" headerRowDxfId="12">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M4:M12">
+    <sortCondition descending="1" ref="M4:M12"/>
+  </sortState>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{5ED47F8B-1F4F-4E7D-B344-B3F657A959A3}" name="Date" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -593,24 +829,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784E7610-A4C1-4EA4-AFAD-75CA6A212B75}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.21875" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -622,9 +859,12 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="M1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -633,183 +873,487 @@
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
+      <c r="B4" s="9">
+        <v>46028</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1">
-        <v>300</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="E4" s="6">
+        <v>15000</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>11</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="M4" s="10">
+        <v>46031</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
+      <c r="B5" s="9">
+        <v>46036</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="6">
+        <v>23000</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="1">
-        <v>400</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="M5" s="10">
+        <v>46030</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="9">
+        <v>46037</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="1">
-        <v>200</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6">
+        <v>500</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="M6" s="10">
+        <v>46029</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>18</v>
+      <c r="B7" s="9">
+        <v>46030</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="1">
-        <v>150</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6">
+        <v>800</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="M7" s="10">
+        <v>46028</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>21</v>
+      <c r="B8" s="9">
+        <v>46027</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6">
         <v>1000</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>22</v>
+      <c r="F8" s="16" t="s">
+        <v>16</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="10">
+        <v>46027</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="9">
+        <v>46029</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="6">
+        <v>2300</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="K9" s="4"/>
+      <c r="M9" s="10">
+        <v>46026</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="9">
+        <v>46031</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="6">
+        <v>100</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="K10" s="4"/>
+      <c r="M10" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9">
+        <v>46032</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="6">
+        <v>300</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="K11" s="4"/>
+      <c r="M11" s="10">
+        <v>46024</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="9">
+        <v>46035</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="6">
+        <v>500</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="K12" s="4"/>
+      <c r="M12" s="9">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="9">
+        <v>46040</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="6">
+        <v>45</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="M13" s="10"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="9">
+        <v>46038</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="6">
+        <v>120</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="9">
+        <v>46026</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="6">
+        <v>150</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="9">
+        <v>46023</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="6">
+        <v>300</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="9">
+        <v>46033</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="6">
+        <v>340</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="9">
+        <v>46039</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="6">
+        <v>370</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="9">
+        <v>46034</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="6">
+        <v>450</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="9">
+        <v>46025</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="6">
+        <v>200</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="1">
-        <v>15000</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>37</v>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="9">
+        <v>46024</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="6">
+        <v>400</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="9"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="9"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <autoFilter ref="D23:D24" xr:uid="{784E7610-A4C1-4EA4-AFAD-75CA6A212B75}"/>
+  <mergeCells count="2">
     <mergeCell ref="A1:I1"/>
+    <mergeCell ref="K8:K12"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>